<commit_message>
update model with new estimates
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\data work\regression_estimates\reg files\revised\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE09CC-A6E4-452D-95E4-6213C84C5B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2EFB6-F4C1-4593-8B5C-4A00789598DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="919" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -624,7 +624,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -648,12 +648,6 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -662,10 +656,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,7 +982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F25AC8-F3A4-45E4-B3D4-29D900575D65}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3606,29 +3605,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="I1" s="18" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4094,29 +4093,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="I1" s="18" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4736,29 +4735,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="I1" s="18" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -5609,13 +5608,13 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="20" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -6811,14 +6810,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D54BEF-A785-4097-B447-1AE751D019CE}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Z25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="2" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -6905,79 +6902,79 @@
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="25">
         <v>-0.14485449357323898</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="25">
         <v>1.7015888845939955E-3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="25">
         <v>1.3725108808073424E-4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="25">
         <v>-2.6240086362088785E-6</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="25">
         <v>-2.8529812070904407E-4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="25">
         <v>-3.4966683432993077E-5</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="25">
         <v>2.2513022650286885E-4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="25">
         <v>1.6434496232809565E-4</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="25">
         <v>-6.3409721327100632E-5</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="25">
         <v>2.255589041279587E-4</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="25">
         <v>1.2464392211008433E-4</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="25">
         <v>2.7406927807089221E-4</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="25">
         <v>-1.8518684056597243E-4</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="25">
         <v>-9.8458545392929222E-5</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="25">
         <v>-4.92546028942822E-5</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="25">
         <v>-3.7153077822145702E-5</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="25">
         <v>-9.3001144039126275E-5</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="25">
         <v>-1.0868280413373638E-4</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="25">
         <v>-2.8142918558288611E-5</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="25">
         <v>-2.1828303530848047E-4</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="25">
         <v>-5.2568673239317739E-4</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="25">
         <v>1.07976708540469E-5</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="25">
         <v>2.7218444335026641E-5</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="25">
         <v>1.1782987276393075E-5</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="25">
         <v>-2.4255406679104512E-3</v>
       </c>
     </row>
@@ -6985,79 +6982,79 @@
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="25">
         <v>-0.65256165499519792</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="25">
         <v>1.3725108808073424E-4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="25">
         <v>2.2927150271831245E-3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="25">
         <v>-4.2857447108404052E-5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="25">
         <v>3.4441864121834143E-4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="25">
         <v>6.6592968666241183E-4</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="25">
         <v>1.2677164207537223E-3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="25">
         <v>6.957704527277668E-4</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="25">
         <v>1.6606149375352538E-4</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="25">
         <v>-4.1434955022574181E-4</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="25">
         <v>-2.2904875698812532E-5</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="25">
         <v>4.3532168754123295E-4</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="25">
         <v>-2.1352013804951629E-5</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="25">
         <v>4.5673190878646724E-4</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="25">
         <v>1.4032546201958682E-4</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="25">
         <v>6.3979834987990675E-5</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="25">
         <v>1.1550199242805646E-4</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="25">
         <v>4.1361036631975406E-5</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="25">
         <v>2.7497061557287249E-4</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="25">
         <v>8.2359504884254794E-5</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="25">
         <v>4.5702769113159861E-4</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="25">
         <v>8.7911573919935426E-4</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="25">
         <v>-1.833638173539074E-4</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="25">
         <v>4.4414555676991507E-5</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="25">
         <v>-3.0680510027793956E-2</v>
       </c>
     </row>
@@ -7065,79 +7062,79 @@
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="25">
         <v>1.0154081768273281E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="25">
         <v>-2.6240086362088785E-6</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="25">
         <v>-4.2857447108404052E-5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="25">
         <v>8.0867294805951264E-7</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="25">
         <v>-4.4233520216489401E-6</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="25">
         <v>-9.6526206298138664E-6</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="25">
         <v>-2.1799796142691885E-5</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="25">
         <v>-1.2063698652978213E-5</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="25">
         <v>-3.2884883732769281E-6</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="25">
         <v>6.8604195917010146E-6</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="25">
         <v>8.2291800761347545E-7</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="25">
         <v>-7.7373455874500793E-6</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="25">
         <v>-3.9390019644404688E-7</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="25">
         <v>-8.4394665840813806E-6</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="25">
         <v>-3.4701541502354965E-6</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="25">
         <v>-1.4380084825889078E-6</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="25">
         <v>-2.8417892568625324E-6</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="25">
         <v>-1.3548108600620792E-6</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="25">
         <v>-5.5418404149012705E-6</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="25">
         <v>-1.9023792491266062E-6</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="25">
         <v>-7.0600482930148543E-6</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="25">
         <v>-1.7066555745213021E-5</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="25">
         <v>2.84427283414986E-6</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="25">
         <v>-8.3754712588214562E-7</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="25">
         <v>5.6750877986327768E-4</v>
       </c>
     </row>
@@ -7145,79 +7142,79 @@
       <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="25">
         <v>-3.9860561668673529E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="25">
         <v>-2.8529812070904407E-4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="25">
         <v>3.4441864121834143E-4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="25">
         <v>-4.4233520216489401E-6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="25">
         <v>3.7815854486860268E-3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="25">
         <v>3.846541429518598E-3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="25">
         <v>-1.1473194610956132E-4</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="25">
         <v>-3.7935510139709087E-4</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="25">
         <v>-1.132608458126678E-4</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="25">
         <v>2.0566487216078379E-4</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="25">
         <v>-3.4815326108692327E-4</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="25">
         <v>-7.3982130363742108E-4</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="25">
         <v>-3.9455552837927587E-4</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="25">
         <v>-5.1583493205040502E-4</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="25">
         <v>-5.8056649943506082E-4</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="25">
         <v>-6.4988495863781441E-4</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="25">
         <v>-4.8872299654842204E-4</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="25">
         <v>-6.4638106503292915E-4</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="25">
         <v>-3.4621956652593254E-4</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="25">
         <v>-3.2919300838930377E-4</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="25">
         <v>2.1329573569200911E-4</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="25">
         <v>-2.8963710510932026E-4</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="25">
         <v>-5.5354307950471453E-4</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="25">
         <v>-8.3055334261009615E-6</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="25">
         <v>-7.3239673226412477E-3</v>
       </c>
     </row>
@@ -7225,79 +7222,79 @@
       <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="25">
         <v>-0.20179529393574946</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="25">
         <v>-3.4966683432993077E-5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="25">
         <v>6.6592968666241183E-4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="25">
         <v>-9.6526206298138664E-6</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="25">
         <v>3.846541429518598E-3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="25">
         <v>1.371312982313953E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="25">
         <v>3.3670986917832689E-5</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="25">
         <v>-2.9798392180914392E-4</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="25">
         <v>-3.6401251366817813E-4</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="25">
         <v>-3.2873699236667971E-4</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="25">
         <v>-4.0525635013890669E-4</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="25">
         <v>-8.0631328520935951E-4</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="25">
         <v>-4.2724001368417571E-4</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="25">
         <v>1.2397587723477076E-3</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="25">
         <v>-6.0815480591771718E-4</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="25">
         <v>-5.0564422485884939E-4</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="25">
         <v>-6.6356398821766649E-4</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="25">
         <v>-9.7025974384637686E-4</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="25">
         <v>-3.4838340834716176E-4</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="25">
         <v>-1.2594232839430348E-4</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="25">
         <v>2.2780275559413678E-4</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="25">
         <v>-1.9135151690613268E-4</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="25">
         <v>-1.1567273185446383E-3</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="25">
         <v>5.6658892155659691E-5</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="25">
         <v>-1.3304483028293707E-2</v>
       </c>
     </row>
@@ -7305,79 +7302,79 @@
       <c r="A7" t="s">
         <v>65</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="25">
         <v>-1.1578010864870911</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="25">
         <v>2.2513022650286885E-4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="25">
         <v>1.2677164207537223E-3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="25">
         <v>-2.1799796142691885E-5</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="25">
         <v>-1.1473194610956132E-4</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="25">
         <v>3.3670986917832689E-5</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="25">
         <v>4.6168274025779159E-3</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="25">
         <v>1.7941097936171333E-3</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="25">
         <v>-3.3762166930549414E-4</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="25">
         <v>2.0736929638190838E-4</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="25">
         <v>5.2812164378885469E-4</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="25">
         <v>9.0840035713587834E-4</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="25">
         <v>-2.1955205549236984E-4</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="25">
         <v>4.8086515101431956E-4</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="25">
         <v>1.2646261871128569E-4</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="25">
         <v>1.7429390795552745E-4</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="25">
         <v>-1.2603814636529659E-4</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="25">
         <v>2.2087620655502922E-4</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="25">
         <v>2.9545317638445743E-4</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="25">
         <v>3.1479709646340011E-5</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="25">
         <v>7.972554861306394E-6</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="25">
         <v>4.521508531641228E-4</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="25">
         <v>-2.024551725107902E-4</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="25">
         <v>1.4277389611808892E-5</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="25">
         <v>-1.8810521777396921E-2</v>
       </c>
     </row>
@@ -7385,79 +7382,79 @@
       <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="25">
         <v>7.6694372644113093E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="25">
         <v>1.6434496232809565E-4</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="25">
         <v>6.957704527277668E-4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="25">
         <v>-1.2063698652978213E-5</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="25">
         <v>-3.7935510139709087E-4</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="25">
         <v>-2.9798392180914392E-4</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="25">
         <v>1.7941097936171333E-3</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="25">
         <v>2.8200293382987822E-3</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="25">
         <v>-2.3223301228248572E-4</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="25">
         <v>-2.5687543034368543E-4</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="25">
         <v>7.115648509085348E-5</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="25">
         <v>2.0148031387138545E-4</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="25">
         <v>-3.180315863220368E-5</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="25">
         <v>4.4916491976963735E-4</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="25">
         <v>3.1629900082423898E-4</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="25">
         <v>2.1849724451546268E-4</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="25">
         <v>1.0291597087540499E-4</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="25">
         <v>3.9227031414154644E-4</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="25">
         <v>3.3071008631440165E-4</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="25">
         <v>1.6367350150356895E-4</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="25">
         <v>-4.1350341070338879E-4</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="25">
         <v>5.7233236843847683E-4</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="25">
         <v>5.9942582227550788E-6</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="25">
         <v>-1.0175843980924783E-5</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="25">
         <v>-1.000691154754238E-2</v>
       </c>
     </row>
@@ -7465,79 +7462,79 @@
       <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="25">
         <v>5.5116860462316578E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="25">
         <v>-6.3409721327100632E-5</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="25">
         <v>1.6606149375352538E-4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="25">
         <v>-3.2884883732769281E-6</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="25">
         <v>-1.132608458126678E-4</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="25">
         <v>-3.6401251366817813E-4</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="25">
         <v>-3.3762166930549414E-4</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="25">
         <v>-2.3223301228248572E-4</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="25">
         <v>4.2476032092709148E-4</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="25">
         <v>-4.7899930912349625E-4</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="25">
         <v>-8.0519748277589609E-5</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="25">
         <v>-6.6461023159518546E-5</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="25">
         <v>7.8073931238424138E-5</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="25">
         <v>2.0245220919571055E-5</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="25">
         <v>1.2032401774755611E-4</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="25">
         <v>1.9010534697422088E-4</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="25">
         <v>1.1708406848232996E-4</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="25">
         <v>8.1619516466128903E-5</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="25">
         <v>1.49209536103706E-4</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="25">
         <v>9.3763771012558286E-5</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="25">
         <v>5.0085707653012876E-4</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="25">
         <v>1.8745047710747162E-5</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="25">
         <v>6.5096399023593845E-5</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="25">
         <v>2.3623460270961116E-6</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="25">
         <v>-2.1529799454289289E-3</v>
       </c>
     </row>
@@ -7545,79 +7542,79 @@
       <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="25">
         <v>-0.14002836163996574</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="25">
         <v>2.255589041279587E-4</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="25">
         <v>-4.1434955022574181E-4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="25">
         <v>6.8604195917010146E-6</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="25">
         <v>2.0566487216078379E-4</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="25">
         <v>-3.2873699236667971E-4</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="25">
         <v>2.0736929638190838E-4</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="25">
         <v>-2.5687543034368543E-4</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="25">
         <v>-4.7899930912349625E-4</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="25">
         <v>4.1614893046690252E-3</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="25">
         <v>9.0690557677783389E-5</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="25">
         <v>-2.531749947291711E-4</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="25">
         <v>-2.7872927074296464E-4</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="25">
         <v>-1.1313804842758035E-4</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="25">
         <v>1.6176235485698242E-4</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="25">
         <v>-3.727105550735603E-4</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="25">
         <v>-3.3095211239885956E-5</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="25">
         <v>1.3147637049267457E-4</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="25">
         <v>-2.5630999749340914E-4</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="25">
         <v>-2.9175042487293026E-4</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="25">
         <v>-1.1622898097649109E-3</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="25">
         <v>2.6599465698443027E-4</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="25">
         <v>-2.5105392201745153E-4</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="25">
         <v>6.3532852139366815E-5</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="25">
         <v>4.6194632338603658E-3</v>
       </c>
     </row>
@@ -7625,79 +7622,79 @@
       <c r="A11" t="s">
         <v>143</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="25">
         <v>-0.34356872387931309</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="25">
         <v>1.2464392211008433E-4</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="25">
         <v>-2.2904875698812532E-5</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="25">
         <v>8.2291800761347545E-7</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="25">
         <v>-3.4815326108692327E-4</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="25">
         <v>-4.0525635013890669E-4</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="25">
         <v>5.2812164378885469E-4</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="25">
         <v>7.115648509085348E-5</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="25">
         <v>-8.0519748277589609E-5</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="25">
         <v>9.0690557677783389E-5</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="25">
         <v>3.340182872152916E-3</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="25">
         <v>2.9646517447074854E-3</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="25">
         <v>-1.0215314727832111E-4</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="25">
         <v>3.0663753233707921E-4</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="25">
         <v>-1.5088823212309858E-5</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="25">
         <v>3.4886846078260978E-5</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="25">
         <v>-1.0200998620716131E-4</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="25">
         <v>-2.1416351897641519E-4</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="25">
         <v>1.8784545213272309E-4</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="25">
         <v>8.4953571662327472E-5</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="25">
         <v>-5.1763065742657546E-5</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="25">
         <v>3.236390033105089E-4</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="25">
         <v>-1.7308567913675455E-5</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="25">
         <v>5.2544842575245703E-6</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="25">
         <v>-2.6379093618582213E-3</v>
       </c>
     </row>
@@ -7705,79 +7702,79 @@
       <c r="A12" t="s">
         <v>144</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="25">
         <v>-0.4098811462231845</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="25">
         <v>2.7406927807089221E-4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="25">
         <v>4.3532168754123295E-4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="25">
         <v>-7.7373455874500793E-6</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="25">
         <v>-7.3982130363742108E-4</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="25">
         <v>-8.0631328520935951E-4</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="25">
         <v>9.0840035713587834E-4</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="25">
         <v>2.0148031387138545E-4</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="25">
         <v>-6.6461023159518546E-5</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="25">
         <v>-2.531749947291711E-4</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="25">
         <v>2.9646517447074854E-3</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="25">
         <v>5.5408195120960971E-3</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="25">
         <v>-9.2543516730859895E-5</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="25">
         <v>9.4435180441856362E-4</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="25">
         <v>-7.6386876494424007E-5</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="25">
         <v>3.0485556520903499E-4</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="25">
         <v>-3.7025456925710259E-5</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="25">
         <v>-9.9787901914152329E-5</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="25">
         <v>5.5712732426393204E-4</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="25">
         <v>2.5638324561553719E-4</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="25">
         <v>5.6443869187169796E-4</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="25">
         <v>1.0032523043572161E-3</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="25">
         <v>-1.8833571180154791E-4</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="25">
         <v>9.1994324071323908E-5</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="25">
         <v>-1.0060455310436799E-2</v>
       </c>
     </row>
@@ -7785,79 +7782,79 @@
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="25">
         <v>8.9930205013640588E-2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="25">
         <v>-1.8518684056597243E-4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="25">
         <v>-2.1352013804951629E-5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="25">
         <v>-3.9390019644404688E-7</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="25">
         <v>-3.9455552837927587E-4</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="25">
         <v>-4.2724001368417571E-4</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="25">
         <v>-2.1955205549236984E-4</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="25">
         <v>-3.180315863220368E-5</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="25">
         <v>7.8073931238424138E-5</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="25">
         <v>-2.7872927074296464E-4</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="25">
         <v>-1.0215314727832111E-4</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="25">
         <v>-9.2543516730859895E-5</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="25">
         <v>1.0146292571219812E-2</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="25">
         <v>3.226694470596658E-3</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="25">
         <v>3.2918368424121307E-3</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="25">
         <v>3.2817683475305798E-3</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="25">
         <v>3.371227717244657E-3</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="25">
         <v>3.3753066561186735E-3</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="25">
         <v>3.2951182613706023E-3</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="25">
         <v>3.3295779594035577E-3</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="25">
         <v>3.4226098569457714E-3</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="25">
         <v>3.2541695135534831E-3</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="25">
         <v>3.3490538446443148E-3</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="25">
         <v>-4.7089675917983181E-5</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="25">
         <v>-1.3951013782035355E-3</v>
       </c>
     </row>
@@ -7865,79 +7862,79 @@
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="25">
         <v>-0.15817571389004698</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="25">
         <v>-9.8458545392929222E-5</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="25">
         <v>4.5673190878646724E-4</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="25">
         <v>-8.4394665840813806E-6</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="25">
         <v>-5.1583493205040502E-4</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="25">
         <v>1.2397587723477076E-3</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="25">
         <v>4.8086515101431956E-4</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="25">
         <v>4.4916491976963735E-4</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="25">
         <v>2.0245220919571055E-5</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="25">
         <v>-1.1313804842758035E-4</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="25">
         <v>3.0663753233707921E-4</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="25">
         <v>9.4435180441856362E-4</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="25">
         <v>3.226694470596658E-3</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="25">
         <v>7.5281210074508312E-3</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="25">
         <v>3.3176864671396467E-3</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="25">
         <v>3.4301050647980963E-3</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="25">
         <v>3.3387812610480134E-3</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="25">
         <v>3.3914644521629133E-3</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="25">
         <v>3.4894830238709628E-3</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="25">
         <v>3.4731375493095413E-3</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="25">
         <v>3.5277572732164862E-3</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="25">
         <v>3.4593586774842844E-3</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="25">
         <v>3.2677651115009384E-3</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="25">
         <v>6.4008303492994029E-5</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="25">
         <v>-1.0453845533536895E-2</v>
       </c>
     </row>
@@ -7945,79 +7942,79 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="25">
         <v>-0.19902974165342746</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="25">
         <v>-4.92546028942822E-5</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="25">
         <v>1.4032546201958682E-4</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="25">
         <v>-3.4701541502354965E-6</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="25">
         <v>-5.8056649943506082E-4</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="25">
         <v>-6.0815480591771718E-4</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="25">
         <v>1.2646261871128569E-4</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="25">
         <v>3.1629900082423898E-4</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="25">
         <v>1.2032401774755611E-4</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="25">
         <v>1.6176235485698242E-4</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="25">
         <v>-1.5088823212309858E-5</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="25">
         <v>-7.6386876494424007E-5</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="25">
         <v>3.2918368424121307E-3</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="25">
         <v>3.3176864671396467E-3</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="25">
         <v>8.0045588315381267E-3</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="25">
         <v>3.2908510281437465E-3</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="25">
         <v>3.3352350461384019E-3</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="25">
         <v>3.3354734077617699E-3</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="25">
         <v>3.2933402446549622E-3</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="25">
         <v>3.2933255184870664E-3</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="25">
         <v>3.4625935230542275E-3</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="25">
         <v>3.2980019206597833E-3</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="25">
         <v>3.301996734873669E-3</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="25">
         <v>1.4735266172636382E-5</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="25">
         <v>-4.5471328425719208E-3</v>
       </c>
     </row>
@@ -8025,79 +8022,79 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="25">
         <v>-0.28635494226982494</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="25">
         <v>-3.7153077822145702E-5</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="25">
         <v>6.3979834987990675E-5</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="25">
         <v>-1.4380084825889078E-6</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="25">
         <v>-6.4988495863781441E-4</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="25">
         <v>-5.0564422485884939E-4</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="25">
         <v>1.7429390795552745E-4</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="25">
         <v>2.1849724451546268E-4</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="25">
         <v>1.9010534697422088E-4</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="25">
         <v>-3.727105550735603E-4</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="25">
         <v>3.4886846078260978E-5</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="25">
         <v>3.0485556520903499E-4</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="25">
         <v>3.2817683475305798E-3</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="25">
         <v>3.4301050647980963E-3</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="25">
         <v>3.2908510281437465E-3</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="25">
         <v>7.6596668569916641E-3</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="25">
         <v>3.3669026740094751E-3</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="25">
         <v>3.3355225602167277E-3</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="25">
         <v>3.3475168744565311E-3</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="25">
         <v>3.3401230030831921E-3</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="25">
         <v>3.6171678624433504E-3</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="25">
         <v>3.4137953517816926E-3</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="25">
         <v>3.3087835698453879E-3</v>
       </c>
-      <c r="Y16">
+      <c r="Y16" s="25">
         <v>-2.0467078196424588E-5</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="25">
         <v>-3.4379843861617326E-3</v>
       </c>
     </row>
@@ -8105,79 +8102,79 @@
       <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="25">
         <v>7.8023757305989802E-2</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="25">
         <v>-9.3001144039126275E-5</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="25">
         <v>1.1550199242805646E-4</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="25">
         <v>-2.8417892568625324E-6</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="25">
         <v>-4.8872299654842204E-4</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="25">
         <v>-6.6356398821766649E-4</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="25">
         <v>-1.2603814636529659E-4</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="25">
         <v>1.0291597087540499E-4</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="25">
         <v>1.1708406848232996E-4</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="25">
         <v>-3.3095211239885956E-5</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="25">
         <v>-1.0200998620716131E-4</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="25">
         <v>-3.7025456925710259E-5</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="25">
         <v>3.371227717244657E-3</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="25">
         <v>3.3387812610480134E-3</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="25">
         <v>3.3352350461384019E-3</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="25">
         <v>3.3669026740094751E-3</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="25">
         <v>7.3060889753039761E-3</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="25">
         <v>3.3778422882468841E-3</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="25">
         <v>3.3516399198216681E-3</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="25">
         <v>3.35423457659801E-3</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="25">
         <v>3.4917165123531562E-3</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="25">
         <v>3.3472958974853804E-3</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="25">
         <v>3.373909773517288E-3</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="25">
         <v>3.2730965582197742E-6</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="25">
         <v>-4.0828555161821281E-3</v>
       </c>
     </row>
@@ -8185,79 +8182,79 @@
       <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="25">
         <v>-0.18873872228131813</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="25">
         <v>-1.0868280413373638E-4</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="25">
         <v>4.1361036631975406E-5</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="25">
         <v>-1.3548108600620792E-6</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="25">
         <v>-6.4638106503292915E-4</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="25">
         <v>-9.7025974384637686E-4</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="25">
         <v>2.2087620655502922E-4</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="25">
         <v>3.9227031414154644E-4</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="25">
         <v>8.1619516466128903E-5</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="25">
         <v>1.3147637049267457E-4</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="25">
         <v>-2.1416351897641519E-4</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="25">
         <v>-9.9787901914152329E-5</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="25">
         <v>3.3753066561186735E-3</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="25">
         <v>3.3914644521629133E-3</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="25">
         <v>3.3354734077617699E-3</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="25">
         <v>3.3355225602167277E-3</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="25">
         <v>3.3778422882468841E-3</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="25">
         <v>7.3969361106132839E-3</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="25">
         <v>3.3604286338967627E-3</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="25">
         <v>3.348802313775494E-3</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="25">
         <v>3.4424434609729875E-3</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="25">
         <v>3.4110281673731977E-3</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="25">
         <v>3.351875032356318E-3</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="25">
         <v>-3.800299097999646E-5</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="25">
         <v>-2.4204761063953001E-3</v>
       </c>
     </row>
@@ -8265,79 +8262,79 @@
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="25">
         <v>-0.15894510601468753</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="25">
         <v>-2.8142918558288611E-5</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="25">
         <v>2.7497061557287249E-4</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="25">
         <v>-5.5418404149012705E-6</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="25">
         <v>-3.4621956652593254E-4</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="25">
         <v>-3.4838340834716176E-4</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="25">
         <v>2.9545317638445743E-4</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="25">
         <v>3.3071008631440165E-4</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="25">
         <v>1.49209536103706E-4</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="25">
         <v>-2.5630999749340914E-4</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="25">
         <v>1.8784545213272309E-4</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="25">
         <v>5.5712732426393204E-4</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="25">
         <v>3.2951182613706023E-3</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="25">
         <v>3.4894830238709628E-3</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="25">
         <v>3.2933402446549622E-3</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="25">
         <v>3.3475168744565311E-3</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="25">
         <v>3.3516399198216681E-3</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="25">
         <v>3.3604286338967627E-3</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="25">
         <v>6.1981482880477234E-3</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="25">
         <v>3.3546112176264138E-3</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="25">
         <v>3.528900972510008E-3</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="25">
         <v>3.4586726185169116E-3</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="25">
         <v>3.227067398844282E-3</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="25">
         <v>-3.0521895668100615E-5</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="25">
         <v>-6.312444501618962E-3</v>
       </c>
     </row>
@@ -8345,79 +8342,79 @@
       <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="25">
         <v>-0.28780619107768368</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="25">
         <v>-2.1828303530848047E-4</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="25">
         <v>8.2359504884254794E-5</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="25">
         <v>-1.9023792491266062E-6</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="25">
         <v>-3.2919300838930377E-4</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="25">
         <v>-1.2594232839430348E-4</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="25">
         <v>3.1479709646340011E-5</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="25">
         <v>1.6367350150356895E-4</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="25">
         <v>9.3763771012558286E-5</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="25">
         <v>-2.9175042487293026E-4</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="25">
         <v>8.4953571662327472E-5</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="25">
         <v>2.5638324561553719E-4</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="25">
         <v>3.3295779594035577E-3</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="25">
         <v>3.4731375493095413E-3</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="25">
         <v>3.2933255184870664E-3</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="25">
         <v>3.3401230030831921E-3</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="25">
         <v>3.35423457659801E-3</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="25">
         <v>3.348802313775494E-3</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="25">
         <v>3.3546112176264138E-3</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="25">
         <v>7.8541748863150702E-3</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="25">
         <v>3.5804828554357559E-3</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="25">
         <v>3.42782437932316E-3</v>
       </c>
-      <c r="X20">
+      <c r="X20" s="25">
         <v>3.2636319204168564E-3</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="25">
         <v>-4.7600812262649602E-6</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="25">
         <v>-3.9597519382081475E-3</v>
       </c>
     </row>
@@ -8425,79 +8422,79 @@
       <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="25">
         <v>-0.17382030825426378</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="25">
         <v>-5.2568673239317739E-4</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="25">
         <v>4.5702769113159861E-4</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="25">
         <v>-7.0600482930148543E-6</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="25">
         <v>2.1329573569200911E-4</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="25">
         <v>2.2780275559413678E-4</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="25">
         <v>7.972554861306394E-6</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="25">
         <v>-4.1350341070338879E-4</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="25">
         <v>5.0085707653012876E-4</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="25">
         <v>-1.1622898097649109E-3</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="25">
         <v>-5.1763065742657546E-5</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="25">
         <v>5.6443869187169796E-4</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="25">
         <v>3.4226098569457714E-3</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="25">
         <v>3.5277572732164862E-3</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="25">
         <v>3.4625935230542275E-3</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="25">
         <v>3.6171678624433504E-3</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="25">
         <v>3.4917165123531562E-3</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="25">
         <v>3.4424434609729875E-3</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="25">
         <v>3.528900972510008E-3</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="25">
         <v>3.5804828554357559E-3</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="25">
         <v>1.8558959688181657E-2</v>
       </c>
-      <c r="W21">
+      <c r="W21" s="25">
         <v>3.426629476958569E-3</v>
       </c>
-      <c r="X21">
+      <c r="X21" s="25">
         <v>3.3742207523942179E-3</v>
       </c>
-      <c r="Y21">
+      <c r="Y21" s="25">
         <v>8.1765511882469477E-5</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="25">
         <v>-1.1587172195334661E-2</v>
       </c>
     </row>
@@ -8505,79 +8502,79 @@
       <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="25">
         <v>0.16497554703951572</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="25">
         <v>1.07976708540469E-5</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="25">
         <v>8.7911573919935426E-4</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="25">
         <v>-1.7066555745213021E-5</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="25">
         <v>-2.8963710510932026E-4</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="25">
         <v>-1.9135151690613268E-4</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="25">
         <v>4.521508531641228E-4</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="25">
         <v>5.7233236843847683E-4</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="25">
         <v>1.8745047710747162E-5</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="25">
         <v>2.6599465698443027E-4</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="25">
         <v>3.236390033105089E-4</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="25">
         <v>1.0032523043572161E-3</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="25">
         <v>3.2541695135534831E-3</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="25">
         <v>3.4593586774842844E-3</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="25">
         <v>3.2980019206597833E-3</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="25">
         <v>3.4137953517816926E-3</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="25">
         <v>3.3472958974853804E-3</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="25">
         <v>3.4110281673731977E-3</v>
       </c>
-      <c r="T22">
+      <c r="T22" s="25">
         <v>3.4586726185169116E-3</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="25">
         <v>3.42782437932316E-3</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="25">
         <v>3.426629476958569E-3</v>
       </c>
-      <c r="W22">
+      <c r="W22" s="25">
         <v>9.558226789450527E-3</v>
       </c>
-      <c r="X22">
+      <c r="X22" s="25">
         <v>3.2517409443712929E-3</v>
       </c>
-      <c r="Y22">
+      <c r="Y22" s="25">
         <v>9.4564107242971378E-5</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="25">
         <v>-1.6126230233396453E-2</v>
       </c>
     </row>
@@ -8585,79 +8582,79 @@
       <c r="A23" t="s">
         <v>54</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="25">
         <v>7.2535872664028556E-2</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="25">
         <v>2.7218444335026641E-5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="25">
         <v>-1.833638173539074E-4</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="25">
         <v>2.84427283414986E-6</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="25">
         <v>-5.5354307950471453E-4</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="25">
         <v>-1.1567273185446383E-3</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="25">
         <v>-2.024551725107902E-4</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="25">
         <v>5.9942582227550788E-6</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="25">
         <v>6.5096399023593845E-5</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="25">
         <v>-2.5105392201745153E-4</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="25">
         <v>-1.7308567913675455E-5</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="25">
         <v>-1.8833571180154791E-4</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="25">
         <v>3.3490538446443148E-3</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="25">
         <v>3.2677651115009384E-3</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="25">
         <v>3.301996734873669E-3</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="25">
         <v>3.3087835698453879E-3</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="25">
         <v>3.373909773517288E-3</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="25">
         <v>3.351875032356318E-3</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="25">
         <v>3.227067398844282E-3</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="25">
         <v>3.2636319204168564E-3</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="25">
         <v>3.3742207523942179E-3</v>
       </c>
-      <c r="W23">
+      <c r="W23" s="25">
         <v>3.2517409443712929E-3</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="25">
         <v>1.0629971708148658E-2</v>
       </c>
-      <c r="Y23">
+      <c r="Y23" s="25">
         <v>1.8382991246653726E-5</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="25">
         <v>-4.3263767816397857E-4</v>
       </c>
     </row>
@@ -8665,79 +8662,79 @@
       <c r="A24" t="s">
         <v>116</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="25">
         <v>5.0938436383108797E-3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="25">
         <v>1.1782987276393075E-5</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="25">
         <v>4.4414555676991507E-5</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="25">
         <v>-8.3754712588214562E-7</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="25">
         <v>-8.3055334261009615E-6</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="25">
         <v>5.6658892155659691E-5</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="25">
         <v>1.4277389611808892E-5</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="25">
         <v>-1.0175843980924783E-5</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="25">
         <v>2.3623460270961116E-6</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="25">
         <v>6.3532852139366815E-5</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="25">
         <v>5.2544842575245703E-6</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="25">
         <v>9.1994324071323908E-5</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="25">
         <v>-4.7089675917983181E-5</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="25">
         <v>6.4008303492994029E-5</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="25">
         <v>1.4735266172636382E-5</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="25">
         <v>-2.0467078196424588E-5</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="25">
         <v>3.2730965582197742E-6</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="25">
         <v>-3.800299097999646E-5</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="25">
         <v>-3.0521895668100615E-5</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="25">
         <v>-4.7600812262649602E-6</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="25">
         <v>8.1765511882469477E-5</v>
       </c>
-      <c r="W24">
+      <c r="W24" s="25">
         <v>9.4564107242971378E-5</v>
       </c>
-      <c r="X24">
+      <c r="X24" s="25">
         <v>1.8382991246653726E-5</v>
       </c>
-      <c r="Y24">
+      <c r="Y24" s="25">
         <v>4.5216905091776519E-5</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="25">
         <v>-1.2948756174171044E-3</v>
       </c>
     </row>
@@ -8745,79 +8742,79 @@
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="25">
         <v>8.2732668862811209</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="25">
         <v>-2.4255406679104512E-3</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="25">
         <v>-3.0680510027793956E-2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="25">
         <v>5.6750877986327768E-4</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="25">
         <v>-7.3239673226412477E-3</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="25">
         <v>-1.3304483028293707E-2</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="25">
         <v>-1.8810521777396921E-2</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="25">
         <v>-1.000691154754238E-2</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="25">
         <v>-2.1529799454289289E-3</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="25">
         <v>4.6194632338603658E-3</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="25">
         <v>-2.6379093618582213E-3</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="25">
         <v>-1.0060455310436799E-2</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="25">
         <v>-1.3951013782035355E-3</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="25">
         <v>-1.0453845533536895E-2</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="25">
         <v>-4.5471328425719208E-3</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="25">
         <v>-3.4379843861617326E-3</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="25">
         <v>-4.0828555161821281E-3</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="25">
         <v>-2.4204761063953001E-3</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="25">
         <v>-6.312444501618962E-3</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="25">
         <v>-3.9597519382081475E-3</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="25">
         <v>-1.1587172195334661E-2</v>
       </c>
-      <c r="W25">
+      <c r="W25" s="25">
         <v>-1.6126230233396453E-2</v>
       </c>
-      <c r="X25">
+      <c r="X25" s="25">
         <v>-4.3263767816397857E-4</v>
       </c>
-      <c r="Y25">
+      <c r="Y25" s="25">
         <v>-1.2948756174171044E-3</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" s="25">
         <v>0.43353698379064198</v>
       </c>
     </row>
@@ -8836,14 +8833,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1285CCF6-ED07-4956-95C1-5161D138438C}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:U20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="21" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -10178,14 +10173,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -10444,16 +10439,16 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="20">
         <v>5.9691530000000004</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="20">
         <v>0.66896920000000004</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="21">
         <v>0</v>
       </c>
     </row>
@@ -10461,7 +10456,7 @@
       <c r="A23" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23">
         <v>16615</v>
       </c>
     </row>
@@ -10469,19 +10464,19 @@
       <c r="A24" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="2">
         <v>0.30330000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="22">
         <v>3.8899999999999997E-2</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -10508,14 +10503,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -10874,16 +10869,16 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="20">
         <v>8.2732670000000006</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="20">
         <v>0.65843529999999995</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="21">
         <v>0</v>
       </c>
     </row>
@@ -10891,7 +10886,7 @@
       <c r="A31" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31">
         <v>96485</v>
       </c>
     </row>
@@ -10899,19 +10894,19 @@
       <c r="A32" t="s">
         <v>134</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="2">
         <v>2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33" s="22">
         <v>0.22309999999999999</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -10937,14 +10932,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>132</v>
       </c>
     </row>
@@ -11189,21 +11184,21 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="20">
         <v>2.4429999999999998E-4</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="20">
         <v>8.3604000000000005E-3</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="21">
         <v>0.03</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" t="s">
         <v>150</v>
       </c>
       <c r="B22" s="2">
@@ -11215,34 +11210,34 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="20">
         <v>27.129180000000002</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="20">
         <v>1.8153790000000001</v>
       </c>
-      <c r="D23" s="23"/>
+      <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24">
         <v>5039</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="22">
         <v>0.3589</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>

</xml_diff>

<commit_message>
resolve minor issues in new model structure
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\data work\regression_estimates\reg files\revised\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2EFB6-F4C1-4593-8B5C-4A00789598DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3196A4D3-8573-4042-ACCC-046101B8864B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="919" activeTab="1" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -29,18 +29,10 @@
     <sheet name="IT_Process E1b - Breaks" sheetId="43" r:id="rId14"/>
     <sheet name="IT_Process E2 - Education Level" sheetId="44" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -519,7 +511,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,16 +530,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -624,7 +606,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -645,9 +627,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -662,7 +642,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,9 +663,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -724,7 +703,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -830,7 +809,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -972,7 +951,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1026,10 +1005,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3605,29 +3584,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="I1" s="24" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4093,29 +4072,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="I1" s="24" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4735,29 +4714,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="I1" s="24" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -5605,10 +5584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED3F4A-E6FE-4140-8298-230560D8220D}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6795,12 +6774,6 @@
         <v>0.44751981756894665</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6808,9 +6781,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D54BEF-A785-4097-B447-1AE751D019CE}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6902,79 +6877,79 @@
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2">
         <v>-0.14485449357323898</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2">
         <v>1.7015888845939955E-3</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2">
         <v>1.3725108808073424E-4</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2">
         <v>-2.6240086362088785E-6</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2">
         <v>-2.8529812070904407E-4</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2">
         <v>-3.4966683432993077E-5</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2">
         <v>2.2513022650286885E-4</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2">
         <v>1.6434496232809565E-4</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2">
         <v>-6.3409721327100632E-5</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2">
         <v>2.255589041279587E-4</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2">
         <v>1.2464392211008433E-4</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2">
         <v>2.7406927807089221E-4</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2">
         <v>-1.8518684056597243E-4</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2">
         <v>-9.8458545392929222E-5</v>
       </c>
-      <c r="P2" s="25">
+      <c r="P2">
         <v>-4.92546028942822E-5</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2">
         <v>-3.7153077822145702E-5</v>
       </c>
-      <c r="R2" s="25">
+      <c r="R2">
         <v>-9.3001144039126275E-5</v>
       </c>
-      <c r="S2" s="25">
+      <c r="S2">
         <v>-1.0868280413373638E-4</v>
       </c>
-      <c r="T2" s="25">
+      <c r="T2">
         <v>-2.8142918558288611E-5</v>
       </c>
-      <c r="U2" s="25">
+      <c r="U2">
         <v>-2.1828303530848047E-4</v>
       </c>
-      <c r="V2" s="25">
+      <c r="V2">
         <v>-5.2568673239317739E-4</v>
       </c>
-      <c r="W2" s="25">
+      <c r="W2">
         <v>1.07976708540469E-5</v>
       </c>
-      <c r="X2" s="25">
+      <c r="X2">
         <v>2.7218444335026641E-5</v>
       </c>
-      <c r="Y2" s="25">
+      <c r="Y2">
         <v>1.1782987276393075E-5</v>
       </c>
-      <c r="Z2" s="25">
+      <c r="Z2">
         <v>-2.4255406679104512E-3</v>
       </c>
     </row>
@@ -6982,79 +6957,79 @@
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3">
         <v>-0.65256165499519792</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3">
         <v>1.3725108808073424E-4</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3">
         <v>2.2927150271831245E-3</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3">
         <v>-4.2857447108404052E-5</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3">
         <v>3.4441864121834143E-4</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3">
         <v>6.6592968666241183E-4</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3">
         <v>1.2677164207537223E-3</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3">
         <v>6.957704527277668E-4</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3">
         <v>1.6606149375352538E-4</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3">
         <v>-4.1434955022574181E-4</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3">
         <v>-2.2904875698812532E-5</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3">
         <v>4.3532168754123295E-4</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3">
         <v>-2.1352013804951629E-5</v>
       </c>
-      <c r="O3" s="25">
+      <c r="O3">
         <v>4.5673190878646724E-4</v>
       </c>
-      <c r="P3" s="25">
+      <c r="P3">
         <v>1.4032546201958682E-4</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3">
         <v>6.3979834987990675E-5</v>
       </c>
-      <c r="R3" s="25">
+      <c r="R3">
         <v>1.1550199242805646E-4</v>
       </c>
-      <c r="S3" s="25">
+      <c r="S3">
         <v>4.1361036631975406E-5</v>
       </c>
-      <c r="T3" s="25">
+      <c r="T3">
         <v>2.7497061557287249E-4</v>
       </c>
-      <c r="U3" s="25">
+      <c r="U3">
         <v>8.2359504884254794E-5</v>
       </c>
-      <c r="V3" s="25">
+      <c r="V3">
         <v>4.5702769113159861E-4</v>
       </c>
-      <c r="W3" s="25">
+      <c r="W3">
         <v>8.7911573919935426E-4</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3">
         <v>-1.833638173539074E-4</v>
       </c>
-      <c r="Y3" s="25">
+      <c r="Y3">
         <v>4.4414555676991507E-5</v>
       </c>
-      <c r="Z3" s="25">
+      <c r="Z3">
         <v>-3.0680510027793956E-2</v>
       </c>
     </row>
@@ -7062,79 +7037,79 @@
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4">
         <v>1.0154081768273281E-2</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4">
         <v>-2.6240086362088785E-6</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4">
         <v>-4.2857447108404052E-5</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4">
         <v>8.0867294805951264E-7</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4">
         <v>-4.4233520216489401E-6</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4">
         <v>-9.6526206298138664E-6</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4">
         <v>-2.1799796142691885E-5</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4">
         <v>-1.2063698652978213E-5</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4">
         <v>-3.2884883732769281E-6</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4">
         <v>6.8604195917010146E-6</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4">
         <v>8.2291800761347545E-7</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4">
         <v>-7.7373455874500793E-6</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4">
         <v>-3.9390019644404688E-7</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4">
         <v>-8.4394665840813806E-6</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4">
         <v>-3.4701541502354965E-6</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4">
         <v>-1.4380084825889078E-6</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4">
         <v>-2.8417892568625324E-6</v>
       </c>
-      <c r="S4" s="25">
+      <c r="S4">
         <v>-1.3548108600620792E-6</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4">
         <v>-5.5418404149012705E-6</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4">
         <v>-1.9023792491266062E-6</v>
       </c>
-      <c r="V4" s="25">
+      <c r="V4">
         <v>-7.0600482930148543E-6</v>
       </c>
-      <c r="W4" s="25">
+      <c r="W4">
         <v>-1.7066555745213021E-5</v>
       </c>
-      <c r="X4" s="25">
+      <c r="X4">
         <v>2.84427283414986E-6</v>
       </c>
-      <c r="Y4" s="25">
+      <c r="Y4">
         <v>-8.3754712588214562E-7</v>
       </c>
-      <c r="Z4" s="25">
+      <c r="Z4">
         <v>5.6750877986327768E-4</v>
       </c>
     </row>
@@ -7142,79 +7117,79 @@
       <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5">
         <v>-3.9860561668673529E-2</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5">
         <v>-2.8529812070904407E-4</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5">
         <v>3.4441864121834143E-4</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5">
         <v>-4.4233520216489401E-6</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5">
         <v>3.7815854486860268E-3</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5">
         <v>3.846541429518598E-3</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5">
         <v>-1.1473194610956132E-4</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5">
         <v>-3.7935510139709087E-4</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5">
         <v>-1.132608458126678E-4</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5">
         <v>2.0566487216078379E-4</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5">
         <v>-3.4815326108692327E-4</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5">
         <v>-7.3982130363742108E-4</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5">
         <v>-3.9455552837927587E-4</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5">
         <v>-5.1583493205040502E-4</v>
       </c>
-      <c r="P5" s="25">
+      <c r="P5">
         <v>-5.8056649943506082E-4</v>
       </c>
-      <c r="Q5" s="25">
+      <c r="Q5">
         <v>-6.4988495863781441E-4</v>
       </c>
-      <c r="R5" s="25">
+      <c r="R5">
         <v>-4.8872299654842204E-4</v>
       </c>
-      <c r="S5" s="25">
+      <c r="S5">
         <v>-6.4638106503292915E-4</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5">
         <v>-3.4621956652593254E-4</v>
       </c>
-      <c r="U5" s="25">
+      <c r="U5">
         <v>-3.2919300838930377E-4</v>
       </c>
-      <c r="V5" s="25">
+      <c r="V5">
         <v>2.1329573569200911E-4</v>
       </c>
-      <c r="W5" s="25">
+      <c r="W5">
         <v>-2.8963710510932026E-4</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5">
         <v>-5.5354307950471453E-4</v>
       </c>
-      <c r="Y5" s="25">
+      <c r="Y5">
         <v>-8.3055334261009615E-6</v>
       </c>
-      <c r="Z5" s="25">
+      <c r="Z5">
         <v>-7.3239673226412477E-3</v>
       </c>
     </row>
@@ -7222,79 +7197,79 @@
       <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6">
         <v>-0.20179529393574946</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6">
         <v>-3.4966683432993077E-5</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6">
         <v>6.6592968666241183E-4</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6">
         <v>-9.6526206298138664E-6</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6">
         <v>3.846541429518598E-3</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6">
         <v>1.371312982313953E-2</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6">
         <v>3.3670986917832689E-5</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6">
         <v>-2.9798392180914392E-4</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6">
         <v>-3.6401251366817813E-4</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6">
         <v>-3.2873699236667971E-4</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6">
         <v>-4.0525635013890669E-4</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6">
         <v>-8.0631328520935951E-4</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6">
         <v>-4.2724001368417571E-4</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6">
         <v>1.2397587723477076E-3</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6">
         <v>-6.0815480591771718E-4</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6">
         <v>-5.0564422485884939E-4</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6">
         <v>-6.6356398821766649E-4</v>
       </c>
-      <c r="S6" s="25">
+      <c r="S6">
         <v>-9.7025974384637686E-4</v>
       </c>
-      <c r="T6" s="25">
+      <c r="T6">
         <v>-3.4838340834716176E-4</v>
       </c>
-      <c r="U6" s="25">
+      <c r="U6">
         <v>-1.2594232839430348E-4</v>
       </c>
-      <c r="V6" s="25">
+      <c r="V6">
         <v>2.2780275559413678E-4</v>
       </c>
-      <c r="W6" s="25">
+      <c r="W6">
         <v>-1.9135151690613268E-4</v>
       </c>
-      <c r="X6" s="25">
+      <c r="X6">
         <v>-1.1567273185446383E-3</v>
       </c>
-      <c r="Y6" s="25">
+      <c r="Y6">
         <v>5.6658892155659691E-5</v>
       </c>
-      <c r="Z6" s="25">
+      <c r="Z6">
         <v>-1.3304483028293707E-2</v>
       </c>
     </row>
@@ -7302,79 +7277,79 @@
       <c r="A7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7">
         <v>-1.1578010864870911</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7">
         <v>2.2513022650286885E-4</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7">
         <v>1.2677164207537223E-3</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7">
         <v>-2.1799796142691885E-5</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7">
         <v>-1.1473194610956132E-4</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7">
         <v>3.3670986917832689E-5</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7">
         <v>4.6168274025779159E-3</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7">
         <v>1.7941097936171333E-3</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7">
         <v>-3.3762166930549414E-4</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7">
         <v>2.0736929638190838E-4</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7">
         <v>5.2812164378885469E-4</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7">
         <v>9.0840035713587834E-4</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7">
         <v>-2.1955205549236984E-4</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7">
         <v>4.8086515101431956E-4</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7">
         <v>1.2646261871128569E-4</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7">
         <v>1.7429390795552745E-4</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7">
         <v>-1.2603814636529659E-4</v>
       </c>
-      <c r="S7" s="25">
+      <c r="S7">
         <v>2.2087620655502922E-4</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7">
         <v>2.9545317638445743E-4</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7">
         <v>3.1479709646340011E-5</v>
       </c>
-      <c r="V7" s="25">
+      <c r="V7">
         <v>7.972554861306394E-6</v>
       </c>
-      <c r="W7" s="25">
+      <c r="W7">
         <v>4.521508531641228E-4</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7">
         <v>-2.024551725107902E-4</v>
       </c>
-      <c r="Y7" s="25">
+      <c r="Y7">
         <v>1.4277389611808892E-5</v>
       </c>
-      <c r="Z7" s="25">
+      <c r="Z7">
         <v>-1.8810521777396921E-2</v>
       </c>
     </row>
@@ -7382,79 +7357,79 @@
       <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8">
         <v>7.6694372644113093E-2</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8">
         <v>1.6434496232809565E-4</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8">
         <v>6.957704527277668E-4</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8">
         <v>-1.2063698652978213E-5</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8">
         <v>-3.7935510139709087E-4</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8">
         <v>-2.9798392180914392E-4</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8">
         <v>1.7941097936171333E-3</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8">
         <v>2.8200293382987822E-3</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8">
         <v>-2.3223301228248572E-4</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8">
         <v>-2.5687543034368543E-4</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8">
         <v>7.115648509085348E-5</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8">
         <v>2.0148031387138545E-4</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8">
         <v>-3.180315863220368E-5</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8">
         <v>4.4916491976963735E-4</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8">
         <v>3.1629900082423898E-4</v>
       </c>
-      <c r="Q8" s="25">
+      <c r="Q8">
         <v>2.1849724451546268E-4</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8">
         <v>1.0291597087540499E-4</v>
       </c>
-      <c r="S8" s="25">
+      <c r="S8">
         <v>3.9227031414154644E-4</v>
       </c>
-      <c r="T8" s="25">
+      <c r="T8">
         <v>3.3071008631440165E-4</v>
       </c>
-      <c r="U8" s="25">
+      <c r="U8">
         <v>1.6367350150356895E-4</v>
       </c>
-      <c r="V8" s="25">
+      <c r="V8">
         <v>-4.1350341070338879E-4</v>
       </c>
-      <c r="W8" s="25">
+      <c r="W8">
         <v>5.7233236843847683E-4</v>
       </c>
-      <c r="X8" s="25">
+      <c r="X8">
         <v>5.9942582227550788E-6</v>
       </c>
-      <c r="Y8" s="25">
+      <c r="Y8">
         <v>-1.0175843980924783E-5</v>
       </c>
-      <c r="Z8" s="25">
+      <c r="Z8">
         <v>-1.000691154754238E-2</v>
       </c>
     </row>
@@ -7462,79 +7437,79 @@
       <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9">
         <v>5.5116860462316578E-2</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9">
         <v>-6.3409721327100632E-5</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9">
         <v>1.6606149375352538E-4</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9">
         <v>-3.2884883732769281E-6</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9">
         <v>-1.132608458126678E-4</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9">
         <v>-3.6401251366817813E-4</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9">
         <v>-3.3762166930549414E-4</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9">
         <v>-2.3223301228248572E-4</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9">
         <v>4.2476032092709148E-4</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9">
         <v>-4.7899930912349625E-4</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9">
         <v>-8.0519748277589609E-5</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9">
         <v>-6.6461023159518546E-5</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9">
         <v>7.8073931238424138E-5</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9">
         <v>2.0245220919571055E-5</v>
       </c>
-      <c r="P9" s="25">
+      <c r="P9">
         <v>1.2032401774755611E-4</v>
       </c>
-      <c r="Q9" s="25">
+      <c r="Q9">
         <v>1.9010534697422088E-4</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9">
         <v>1.1708406848232996E-4</v>
       </c>
-      <c r="S9" s="25">
+      <c r="S9">
         <v>8.1619516466128903E-5</v>
       </c>
-      <c r="T9" s="25">
+      <c r="T9">
         <v>1.49209536103706E-4</v>
       </c>
-      <c r="U9" s="25">
+      <c r="U9">
         <v>9.3763771012558286E-5</v>
       </c>
-      <c r="V9" s="25">
+      <c r="V9">
         <v>5.0085707653012876E-4</v>
       </c>
-      <c r="W9" s="25">
+      <c r="W9">
         <v>1.8745047710747162E-5</v>
       </c>
-      <c r="X9" s="25">
+      <c r="X9">
         <v>6.5096399023593845E-5</v>
       </c>
-      <c r="Y9" s="25">
+      <c r="Y9">
         <v>2.3623460270961116E-6</v>
       </c>
-      <c r="Z9" s="25">
+      <c r="Z9">
         <v>-2.1529799454289289E-3</v>
       </c>
     </row>
@@ -7542,79 +7517,79 @@
       <c r="A10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10">
         <v>-0.14002836163996574</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10">
         <v>2.255589041279587E-4</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10">
         <v>-4.1434955022574181E-4</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10">
         <v>6.8604195917010146E-6</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10">
         <v>2.0566487216078379E-4</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10">
         <v>-3.2873699236667971E-4</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10">
         <v>2.0736929638190838E-4</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10">
         <v>-2.5687543034368543E-4</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10">
         <v>-4.7899930912349625E-4</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10">
         <v>4.1614893046690252E-3</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10">
         <v>9.0690557677783389E-5</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10">
         <v>-2.531749947291711E-4</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10">
         <v>-2.7872927074296464E-4</v>
       </c>
-      <c r="O10" s="25">
+      <c r="O10">
         <v>-1.1313804842758035E-4</v>
       </c>
-      <c r="P10" s="25">
+      <c r="P10">
         <v>1.6176235485698242E-4</v>
       </c>
-      <c r="Q10" s="25">
+      <c r="Q10">
         <v>-3.727105550735603E-4</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10">
         <v>-3.3095211239885956E-5</v>
       </c>
-      <c r="S10" s="25">
+      <c r="S10">
         <v>1.3147637049267457E-4</v>
       </c>
-      <c r="T10" s="25">
+      <c r="T10">
         <v>-2.5630999749340914E-4</v>
       </c>
-      <c r="U10" s="25">
+      <c r="U10">
         <v>-2.9175042487293026E-4</v>
       </c>
-      <c r="V10" s="25">
+      <c r="V10">
         <v>-1.1622898097649109E-3</v>
       </c>
-      <c r="W10" s="25">
+      <c r="W10">
         <v>2.6599465698443027E-4</v>
       </c>
-      <c r="X10" s="25">
+      <c r="X10">
         <v>-2.5105392201745153E-4</v>
       </c>
-      <c r="Y10" s="25">
+      <c r="Y10">
         <v>6.3532852139366815E-5</v>
       </c>
-      <c r="Z10" s="25">
+      <c r="Z10">
         <v>4.6194632338603658E-3</v>
       </c>
     </row>
@@ -7622,79 +7597,79 @@
       <c r="A11" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11">
         <v>-0.34356872387931309</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11">
         <v>1.2464392211008433E-4</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11">
         <v>-2.2904875698812532E-5</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11">
         <v>8.2291800761347545E-7</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11">
         <v>-3.4815326108692327E-4</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11">
         <v>-4.0525635013890669E-4</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11">
         <v>5.2812164378885469E-4</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11">
         <v>7.115648509085348E-5</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11">
         <v>-8.0519748277589609E-5</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11">
         <v>9.0690557677783389E-5</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11">
         <v>3.340182872152916E-3</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11">
         <v>2.9646517447074854E-3</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11">
         <v>-1.0215314727832111E-4</v>
       </c>
-      <c r="O11" s="25">
+      <c r="O11">
         <v>3.0663753233707921E-4</v>
       </c>
-      <c r="P11" s="25">
+      <c r="P11">
         <v>-1.5088823212309858E-5</v>
       </c>
-      <c r="Q11" s="25">
+      <c r="Q11">
         <v>3.4886846078260978E-5</v>
       </c>
-      <c r="R11" s="25">
+      <c r="R11">
         <v>-1.0200998620716131E-4</v>
       </c>
-      <c r="S11" s="25">
+      <c r="S11">
         <v>-2.1416351897641519E-4</v>
       </c>
-      <c r="T11" s="25">
+      <c r="T11">
         <v>1.8784545213272309E-4</v>
       </c>
-      <c r="U11" s="25">
+      <c r="U11">
         <v>8.4953571662327472E-5</v>
       </c>
-      <c r="V11" s="25">
+      <c r="V11">
         <v>-5.1763065742657546E-5</v>
       </c>
-      <c r="W11" s="25">
+      <c r="W11">
         <v>3.236390033105089E-4</v>
       </c>
-      <c r="X11" s="25">
+      <c r="X11">
         <v>-1.7308567913675455E-5</v>
       </c>
-      <c r="Y11" s="25">
+      <c r="Y11">
         <v>5.2544842575245703E-6</v>
       </c>
-      <c r="Z11" s="25">
+      <c r="Z11">
         <v>-2.6379093618582213E-3</v>
       </c>
     </row>
@@ -7702,79 +7677,79 @@
       <c r="A12" t="s">
         <v>144</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12">
         <v>-0.4098811462231845</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12">
         <v>2.7406927807089221E-4</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12">
         <v>4.3532168754123295E-4</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12">
         <v>-7.7373455874500793E-6</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12">
         <v>-7.3982130363742108E-4</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12">
         <v>-8.0631328520935951E-4</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12">
         <v>9.0840035713587834E-4</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12">
         <v>2.0148031387138545E-4</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12">
         <v>-6.6461023159518546E-5</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12">
         <v>-2.531749947291711E-4</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12">
         <v>2.9646517447074854E-3</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12">
         <v>5.5408195120960971E-3</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12">
         <v>-9.2543516730859895E-5</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12">
         <v>9.4435180441856362E-4</v>
       </c>
-      <c r="P12" s="25">
+      <c r="P12">
         <v>-7.6386876494424007E-5</v>
       </c>
-      <c r="Q12" s="25">
+      <c r="Q12">
         <v>3.0485556520903499E-4</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12">
         <v>-3.7025456925710259E-5</v>
       </c>
-      <c r="S12" s="25">
+      <c r="S12">
         <v>-9.9787901914152329E-5</v>
       </c>
-      <c r="T12" s="25">
+      <c r="T12">
         <v>5.5712732426393204E-4</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12">
         <v>2.5638324561553719E-4</v>
       </c>
-      <c r="V12" s="25">
+      <c r="V12">
         <v>5.6443869187169796E-4</v>
       </c>
-      <c r="W12" s="25">
+      <c r="W12">
         <v>1.0032523043572161E-3</v>
       </c>
-      <c r="X12" s="25">
+      <c r="X12">
         <v>-1.8833571180154791E-4</v>
       </c>
-      <c r="Y12" s="25">
+      <c r="Y12">
         <v>9.1994324071323908E-5</v>
       </c>
-      <c r="Z12" s="25">
+      <c r="Z12">
         <v>-1.0060455310436799E-2</v>
       </c>
     </row>
@@ -7782,79 +7757,79 @@
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13">
         <v>8.9930205013640588E-2</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13">
         <v>-1.8518684056597243E-4</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13">
         <v>-2.1352013804951629E-5</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13">
         <v>-3.9390019644404688E-7</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13">
         <v>-3.9455552837927587E-4</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13">
         <v>-4.2724001368417571E-4</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13">
         <v>-2.1955205549236984E-4</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13">
         <v>-3.180315863220368E-5</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13">
         <v>7.8073931238424138E-5</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13">
         <v>-2.7872927074296464E-4</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13">
         <v>-1.0215314727832111E-4</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13">
         <v>-9.2543516730859895E-5</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13">
         <v>1.0146292571219812E-2</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13">
         <v>3.226694470596658E-3</v>
       </c>
-      <c r="P13" s="25">
+      <c r="P13">
         <v>3.2918368424121307E-3</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13">
         <v>3.2817683475305798E-3</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13">
         <v>3.371227717244657E-3</v>
       </c>
-      <c r="S13" s="25">
+      <c r="S13">
         <v>3.3753066561186735E-3</v>
       </c>
-      <c r="T13" s="25">
+      <c r="T13">
         <v>3.2951182613706023E-3</v>
       </c>
-      <c r="U13" s="25">
+      <c r="U13">
         <v>3.3295779594035577E-3</v>
       </c>
-      <c r="V13" s="25">
+      <c r="V13">
         <v>3.4226098569457714E-3</v>
       </c>
-      <c r="W13" s="25">
+      <c r="W13">
         <v>3.2541695135534831E-3</v>
       </c>
-      <c r="X13" s="25">
+      <c r="X13">
         <v>3.3490538446443148E-3</v>
       </c>
-      <c r="Y13" s="25">
+      <c r="Y13">
         <v>-4.7089675917983181E-5</v>
       </c>
-      <c r="Z13" s="25">
+      <c r="Z13">
         <v>-1.3951013782035355E-3</v>
       </c>
     </row>
@@ -7862,79 +7837,79 @@
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14">
         <v>-0.15817571389004698</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14">
         <v>-9.8458545392929222E-5</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14">
         <v>4.5673190878646724E-4</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14">
         <v>-8.4394665840813806E-6</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14">
         <v>-5.1583493205040502E-4</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14">
         <v>1.2397587723477076E-3</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14">
         <v>4.8086515101431956E-4</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14">
         <v>4.4916491976963735E-4</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14">
         <v>2.0245220919571055E-5</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14">
         <v>-1.1313804842758035E-4</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14">
         <v>3.0663753233707921E-4</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14">
         <v>9.4435180441856362E-4</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14">
         <v>3.226694470596658E-3</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14">
         <v>7.5281210074508312E-3</v>
       </c>
-      <c r="P14" s="25">
+      <c r="P14">
         <v>3.3176864671396467E-3</v>
       </c>
-      <c r="Q14" s="25">
+      <c r="Q14">
         <v>3.4301050647980963E-3</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14">
         <v>3.3387812610480134E-3</v>
       </c>
-      <c r="S14" s="25">
+      <c r="S14">
         <v>3.3914644521629133E-3</v>
       </c>
-      <c r="T14" s="25">
+      <c r="T14">
         <v>3.4894830238709628E-3</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14">
         <v>3.4731375493095413E-3</v>
       </c>
-      <c r="V14" s="25">
+      <c r="V14">
         <v>3.5277572732164862E-3</v>
       </c>
-      <c r="W14" s="25">
+      <c r="W14">
         <v>3.4593586774842844E-3</v>
       </c>
-      <c r="X14" s="25">
+      <c r="X14">
         <v>3.2677651115009384E-3</v>
       </c>
-      <c r="Y14" s="25">
+      <c r="Y14">
         <v>6.4008303492994029E-5</v>
       </c>
-      <c r="Z14" s="25">
+      <c r="Z14">
         <v>-1.0453845533536895E-2</v>
       </c>
     </row>
@@ -7942,79 +7917,79 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15">
         <v>-0.19902974165342746</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15">
         <v>-4.92546028942822E-5</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15">
         <v>1.4032546201958682E-4</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15">
         <v>-3.4701541502354965E-6</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15">
         <v>-5.8056649943506082E-4</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15">
         <v>-6.0815480591771718E-4</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15">
         <v>1.2646261871128569E-4</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15">
         <v>3.1629900082423898E-4</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15">
         <v>1.2032401774755611E-4</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15">
         <v>1.6176235485698242E-4</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15">
         <v>-1.5088823212309858E-5</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15">
         <v>-7.6386876494424007E-5</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15">
         <v>3.2918368424121307E-3</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15">
         <v>3.3176864671396467E-3</v>
       </c>
-      <c r="P15" s="25">
+      <c r="P15">
         <v>8.0045588315381267E-3</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15">
         <v>3.2908510281437465E-3</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15">
         <v>3.3352350461384019E-3</v>
       </c>
-      <c r="S15" s="25">
+      <c r="S15">
         <v>3.3354734077617699E-3</v>
       </c>
-      <c r="T15" s="25">
+      <c r="T15">
         <v>3.2933402446549622E-3</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15">
         <v>3.2933255184870664E-3</v>
       </c>
-      <c r="V15" s="25">
+      <c r="V15">
         <v>3.4625935230542275E-3</v>
       </c>
-      <c r="W15" s="25">
+      <c r="W15">
         <v>3.2980019206597833E-3</v>
       </c>
-      <c r="X15" s="25">
+      <c r="X15">
         <v>3.301996734873669E-3</v>
       </c>
-      <c r="Y15" s="25">
+      <c r="Y15">
         <v>1.4735266172636382E-5</v>
       </c>
-      <c r="Z15" s="25">
+      <c r="Z15">
         <v>-4.5471328425719208E-3</v>
       </c>
     </row>
@@ -8022,79 +7997,79 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16">
         <v>-0.28635494226982494</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16">
         <v>-3.7153077822145702E-5</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16">
         <v>6.3979834987990675E-5</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16">
         <v>-1.4380084825889078E-6</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16">
         <v>-6.4988495863781441E-4</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16">
         <v>-5.0564422485884939E-4</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16">
         <v>1.7429390795552745E-4</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16">
         <v>2.1849724451546268E-4</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16">
         <v>1.9010534697422088E-4</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16">
         <v>-3.727105550735603E-4</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16">
         <v>3.4886846078260978E-5</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16">
         <v>3.0485556520903499E-4</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16">
         <v>3.2817683475305798E-3</v>
       </c>
-      <c r="O16" s="25">
+      <c r="O16">
         <v>3.4301050647980963E-3</v>
       </c>
-      <c r="P16" s="25">
+      <c r="P16">
         <v>3.2908510281437465E-3</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16">
         <v>7.6596668569916641E-3</v>
       </c>
-      <c r="R16" s="25">
+      <c r="R16">
         <v>3.3669026740094751E-3</v>
       </c>
-      <c r="S16" s="25">
+      <c r="S16">
         <v>3.3355225602167277E-3</v>
       </c>
-      <c r="T16" s="25">
+      <c r="T16">
         <v>3.3475168744565311E-3</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16">
         <v>3.3401230030831921E-3</v>
       </c>
-      <c r="V16" s="25">
+      <c r="V16">
         <v>3.6171678624433504E-3</v>
       </c>
-      <c r="W16" s="25">
+      <c r="W16">
         <v>3.4137953517816926E-3</v>
       </c>
-      <c r="X16" s="25">
+      <c r="X16">
         <v>3.3087835698453879E-3</v>
       </c>
-      <c r="Y16" s="25">
+      <c r="Y16">
         <v>-2.0467078196424588E-5</v>
       </c>
-      <c r="Z16" s="25">
+      <c r="Z16">
         <v>-3.4379843861617326E-3</v>
       </c>
     </row>
@@ -8102,79 +8077,79 @@
       <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17">
         <v>7.8023757305989802E-2</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17">
         <v>-9.3001144039126275E-5</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17">
         <v>1.1550199242805646E-4</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17">
         <v>-2.8417892568625324E-6</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17">
         <v>-4.8872299654842204E-4</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17">
         <v>-6.6356398821766649E-4</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17">
         <v>-1.2603814636529659E-4</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17">
         <v>1.0291597087540499E-4</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17">
         <v>1.1708406848232996E-4</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17">
         <v>-3.3095211239885956E-5</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17">
         <v>-1.0200998620716131E-4</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17">
         <v>-3.7025456925710259E-5</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17">
         <v>3.371227717244657E-3</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17">
         <v>3.3387812610480134E-3</v>
       </c>
-      <c r="P17" s="25">
+      <c r="P17">
         <v>3.3352350461384019E-3</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17">
         <v>3.3669026740094751E-3</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17">
         <v>7.3060889753039761E-3</v>
       </c>
-      <c r="S17" s="25">
+      <c r="S17">
         <v>3.3778422882468841E-3</v>
       </c>
-      <c r="T17" s="25">
+      <c r="T17">
         <v>3.3516399198216681E-3</v>
       </c>
-      <c r="U17" s="25">
+      <c r="U17">
         <v>3.35423457659801E-3</v>
       </c>
-      <c r="V17" s="25">
+      <c r="V17">
         <v>3.4917165123531562E-3</v>
       </c>
-      <c r="W17" s="25">
+      <c r="W17">
         <v>3.3472958974853804E-3</v>
       </c>
-      <c r="X17" s="25">
+      <c r="X17">
         <v>3.373909773517288E-3</v>
       </c>
-      <c r="Y17" s="25">
+      <c r="Y17">
         <v>3.2730965582197742E-6</v>
       </c>
-      <c r="Z17" s="25">
+      <c r="Z17">
         <v>-4.0828555161821281E-3</v>
       </c>
     </row>
@@ -8182,79 +8157,79 @@
       <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18">
         <v>-0.18873872228131813</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18">
         <v>-1.0868280413373638E-4</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18">
         <v>4.1361036631975406E-5</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18">
         <v>-1.3548108600620792E-6</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18">
         <v>-6.4638106503292915E-4</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18">
         <v>-9.7025974384637686E-4</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18">
         <v>2.2087620655502922E-4</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18">
         <v>3.9227031414154644E-4</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18">
         <v>8.1619516466128903E-5</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18">
         <v>1.3147637049267457E-4</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18">
         <v>-2.1416351897641519E-4</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18">
         <v>-9.9787901914152329E-5</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18">
         <v>3.3753066561186735E-3</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18">
         <v>3.3914644521629133E-3</v>
       </c>
-      <c r="P18" s="25">
+      <c r="P18">
         <v>3.3354734077617699E-3</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18">
         <v>3.3355225602167277E-3</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18">
         <v>3.3778422882468841E-3</v>
       </c>
-      <c r="S18" s="25">
+      <c r="S18">
         <v>7.3969361106132839E-3</v>
       </c>
-      <c r="T18" s="25">
+      <c r="T18">
         <v>3.3604286338967627E-3</v>
       </c>
-      <c r="U18" s="25">
+      <c r="U18">
         <v>3.348802313775494E-3</v>
       </c>
-      <c r="V18" s="25">
+      <c r="V18">
         <v>3.4424434609729875E-3</v>
       </c>
-      <c r="W18" s="25">
+      <c r="W18">
         <v>3.4110281673731977E-3</v>
       </c>
-      <c r="X18" s="25">
+      <c r="X18">
         <v>3.351875032356318E-3</v>
       </c>
-      <c r="Y18" s="25">
+      <c r="Y18">
         <v>-3.800299097999646E-5</v>
       </c>
-      <c r="Z18" s="25">
+      <c r="Z18">
         <v>-2.4204761063953001E-3</v>
       </c>
     </row>
@@ -8262,79 +8237,79 @@
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19">
         <v>-0.15894510601468753</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19">
         <v>-2.8142918558288611E-5</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19">
         <v>2.7497061557287249E-4</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19">
         <v>-5.5418404149012705E-6</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19">
         <v>-3.4621956652593254E-4</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19">
         <v>-3.4838340834716176E-4</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19">
         <v>2.9545317638445743E-4</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19">
         <v>3.3071008631440165E-4</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19">
         <v>1.49209536103706E-4</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19">
         <v>-2.5630999749340914E-4</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19">
         <v>1.8784545213272309E-4</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19">
         <v>5.5712732426393204E-4</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19">
         <v>3.2951182613706023E-3</v>
       </c>
-      <c r="O19" s="25">
+      <c r="O19">
         <v>3.4894830238709628E-3</v>
       </c>
-      <c r="P19" s="25">
+      <c r="P19">
         <v>3.2933402446549622E-3</v>
       </c>
-      <c r="Q19" s="25">
+      <c r="Q19">
         <v>3.3475168744565311E-3</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19">
         <v>3.3516399198216681E-3</v>
       </c>
-      <c r="S19" s="25">
+      <c r="S19">
         <v>3.3604286338967627E-3</v>
       </c>
-      <c r="T19" s="25">
+      <c r="T19">
         <v>6.1981482880477234E-3</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19">
         <v>3.3546112176264138E-3</v>
       </c>
-      <c r="V19" s="25">
+      <c r="V19">
         <v>3.528900972510008E-3</v>
       </c>
-      <c r="W19" s="25">
+      <c r="W19">
         <v>3.4586726185169116E-3</v>
       </c>
-      <c r="X19" s="25">
+      <c r="X19">
         <v>3.227067398844282E-3</v>
       </c>
-      <c r="Y19" s="25">
+      <c r="Y19">
         <v>-3.0521895668100615E-5</v>
       </c>
-      <c r="Z19" s="25">
+      <c r="Z19">
         <v>-6.312444501618962E-3</v>
       </c>
     </row>
@@ -8342,79 +8317,79 @@
       <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20">
         <v>-0.28780619107768368</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20">
         <v>-2.1828303530848047E-4</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20">
         <v>8.2359504884254794E-5</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20">
         <v>-1.9023792491266062E-6</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20">
         <v>-3.2919300838930377E-4</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20">
         <v>-1.2594232839430348E-4</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20">
         <v>3.1479709646340011E-5</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20">
         <v>1.6367350150356895E-4</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20">
         <v>9.3763771012558286E-5</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20">
         <v>-2.9175042487293026E-4</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20">
         <v>8.4953571662327472E-5</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20">
         <v>2.5638324561553719E-4</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20">
         <v>3.3295779594035577E-3</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20">
         <v>3.4731375493095413E-3</v>
       </c>
-      <c r="P20" s="25">
+      <c r="P20">
         <v>3.2933255184870664E-3</v>
       </c>
-      <c r="Q20" s="25">
+      <c r="Q20">
         <v>3.3401230030831921E-3</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20">
         <v>3.35423457659801E-3</v>
       </c>
-      <c r="S20" s="25">
+      <c r="S20">
         <v>3.348802313775494E-3</v>
       </c>
-      <c r="T20" s="25">
+      <c r="T20">
         <v>3.3546112176264138E-3</v>
       </c>
-      <c r="U20" s="25">
+      <c r="U20">
         <v>7.8541748863150702E-3</v>
       </c>
-      <c r="V20" s="25">
+      <c r="V20">
         <v>3.5804828554357559E-3</v>
       </c>
-      <c r="W20" s="25">
+      <c r="W20">
         <v>3.42782437932316E-3</v>
       </c>
-      <c r="X20" s="25">
+      <c r="X20">
         <v>3.2636319204168564E-3</v>
       </c>
-      <c r="Y20" s="25">
+      <c r="Y20">
         <v>-4.7600812262649602E-6</v>
       </c>
-      <c r="Z20" s="25">
+      <c r="Z20">
         <v>-3.9597519382081475E-3</v>
       </c>
     </row>
@@ -8422,79 +8397,79 @@
       <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21">
         <v>-0.17382030825426378</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21">
         <v>-5.2568673239317739E-4</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21">
         <v>4.5702769113159861E-4</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21">
         <v>-7.0600482930148543E-6</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21">
         <v>2.1329573569200911E-4</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21">
         <v>2.2780275559413678E-4</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21">
         <v>7.972554861306394E-6</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21">
         <v>-4.1350341070338879E-4</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21">
         <v>5.0085707653012876E-4</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21">
         <v>-1.1622898097649109E-3</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21">
         <v>-5.1763065742657546E-5</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21">
         <v>5.6443869187169796E-4</v>
       </c>
-      <c r="N21" s="25">
+      <c r="N21">
         <v>3.4226098569457714E-3</v>
       </c>
-      <c r="O21" s="25">
+      <c r="O21">
         <v>3.5277572732164862E-3</v>
       </c>
-      <c r="P21" s="25">
+      <c r="P21">
         <v>3.4625935230542275E-3</v>
       </c>
-      <c r="Q21" s="25">
+      <c r="Q21">
         <v>3.6171678624433504E-3</v>
       </c>
-      <c r="R21" s="25">
+      <c r="R21">
         <v>3.4917165123531562E-3</v>
       </c>
-      <c r="S21" s="25">
+      <c r="S21">
         <v>3.4424434609729875E-3</v>
       </c>
-      <c r="T21" s="25">
+      <c r="T21">
         <v>3.528900972510008E-3</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21">
         <v>3.5804828554357559E-3</v>
       </c>
-      <c r="V21" s="25">
+      <c r="V21">
         <v>1.8558959688181657E-2</v>
       </c>
-      <c r="W21" s="25">
+      <c r="W21">
         <v>3.426629476958569E-3</v>
       </c>
-      <c r="X21" s="25">
+      <c r="X21">
         <v>3.3742207523942179E-3</v>
       </c>
-      <c r="Y21" s="25">
+      <c r="Y21">
         <v>8.1765511882469477E-5</v>
       </c>
-      <c r="Z21" s="25">
+      <c r="Z21">
         <v>-1.1587172195334661E-2</v>
       </c>
     </row>
@@ -8502,79 +8477,79 @@
       <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22">
         <v>0.16497554703951572</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22">
         <v>1.07976708540469E-5</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22">
         <v>8.7911573919935426E-4</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22">
         <v>-1.7066555745213021E-5</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22">
         <v>-2.8963710510932026E-4</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22">
         <v>-1.9135151690613268E-4</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22">
         <v>4.521508531641228E-4</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22">
         <v>5.7233236843847683E-4</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22">
         <v>1.8745047710747162E-5</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22">
         <v>2.6599465698443027E-4</v>
       </c>
-      <c r="L22" s="25">
+      <c r="L22">
         <v>3.236390033105089E-4</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22">
         <v>1.0032523043572161E-3</v>
       </c>
-      <c r="N22" s="25">
+      <c r="N22">
         <v>3.2541695135534831E-3</v>
       </c>
-      <c r="O22" s="25">
+      <c r="O22">
         <v>3.4593586774842844E-3</v>
       </c>
-      <c r="P22" s="25">
+      <c r="P22">
         <v>3.2980019206597833E-3</v>
       </c>
-      <c r="Q22" s="25">
+      <c r="Q22">
         <v>3.4137953517816926E-3</v>
       </c>
-      <c r="R22" s="25">
+      <c r="R22">
         <v>3.3472958974853804E-3</v>
       </c>
-      <c r="S22" s="25">
+      <c r="S22">
         <v>3.4110281673731977E-3</v>
       </c>
-      <c r="T22" s="25">
+      <c r="T22">
         <v>3.4586726185169116E-3</v>
       </c>
-      <c r="U22" s="25">
+      <c r="U22">
         <v>3.42782437932316E-3</v>
       </c>
-      <c r="V22" s="25">
+      <c r="V22">
         <v>3.426629476958569E-3</v>
       </c>
-      <c r="W22" s="25">
+      <c r="W22">
         <v>9.558226789450527E-3</v>
       </c>
-      <c r="X22" s="25">
+      <c r="X22">
         <v>3.2517409443712929E-3</v>
       </c>
-      <c r="Y22" s="25">
+      <c r="Y22">
         <v>9.4564107242971378E-5</v>
       </c>
-      <c r="Z22" s="25">
+      <c r="Z22">
         <v>-1.6126230233396453E-2</v>
       </c>
     </row>
@@ -8582,79 +8557,79 @@
       <c r="A23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23">
         <v>7.2535872664028556E-2</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23">
         <v>2.7218444335026641E-5</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23">
         <v>-1.833638173539074E-4</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23">
         <v>2.84427283414986E-6</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23">
         <v>-5.5354307950471453E-4</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23">
         <v>-1.1567273185446383E-3</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23">
         <v>-2.024551725107902E-4</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23">
         <v>5.9942582227550788E-6</v>
       </c>
-      <c r="J23" s="25">
+      <c r="J23">
         <v>6.5096399023593845E-5</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23">
         <v>-2.5105392201745153E-4</v>
       </c>
-      <c r="L23" s="25">
+      <c r="L23">
         <v>-1.7308567913675455E-5</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23">
         <v>-1.8833571180154791E-4</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23">
         <v>3.3490538446443148E-3</v>
       </c>
-      <c r="O23" s="25">
+      <c r="O23">
         <v>3.2677651115009384E-3</v>
       </c>
-      <c r="P23" s="25">
+      <c r="P23">
         <v>3.301996734873669E-3</v>
       </c>
-      <c r="Q23" s="25">
+      <c r="Q23">
         <v>3.3087835698453879E-3</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R23">
         <v>3.373909773517288E-3</v>
       </c>
-      <c r="S23" s="25">
+      <c r="S23">
         <v>3.351875032356318E-3</v>
       </c>
-      <c r="T23" s="25">
+      <c r="T23">
         <v>3.227067398844282E-3</v>
       </c>
-      <c r="U23" s="25">
+      <c r="U23">
         <v>3.2636319204168564E-3</v>
       </c>
-      <c r="V23" s="25">
+      <c r="V23">
         <v>3.3742207523942179E-3</v>
       </c>
-      <c r="W23" s="25">
+      <c r="W23">
         <v>3.2517409443712929E-3</v>
       </c>
-      <c r="X23" s="25">
+      <c r="X23">
         <v>1.0629971708148658E-2</v>
       </c>
-      <c r="Y23" s="25">
+      <c r="Y23">
         <v>1.8382991246653726E-5</v>
       </c>
-      <c r="Z23" s="25">
+      <c r="Z23">
         <v>-4.3263767816397857E-4</v>
       </c>
     </row>
@@ -8662,79 +8637,79 @@
       <c r="A24" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24">
         <v>5.0938436383108797E-3</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24">
         <v>1.1782987276393075E-5</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24">
         <v>4.4414555676991507E-5</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24">
         <v>-8.3754712588214562E-7</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24">
         <v>-8.3055334261009615E-6</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24">
         <v>5.6658892155659691E-5</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24">
         <v>1.4277389611808892E-5</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24">
         <v>-1.0175843980924783E-5</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24">
         <v>2.3623460270961116E-6</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24">
         <v>6.3532852139366815E-5</v>
       </c>
-      <c r="L24" s="25">
+      <c r="L24">
         <v>5.2544842575245703E-6</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24">
         <v>9.1994324071323908E-5</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24">
         <v>-4.7089675917983181E-5</v>
       </c>
-      <c r="O24" s="25">
+      <c r="O24">
         <v>6.4008303492994029E-5</v>
       </c>
-      <c r="P24" s="25">
+      <c r="P24">
         <v>1.4735266172636382E-5</v>
       </c>
-      <c r="Q24" s="25">
+      <c r="Q24">
         <v>-2.0467078196424588E-5</v>
       </c>
-      <c r="R24" s="25">
+      <c r="R24">
         <v>3.2730965582197742E-6</v>
       </c>
-      <c r="S24" s="25">
+      <c r="S24">
         <v>-3.800299097999646E-5</v>
       </c>
-      <c r="T24" s="25">
+      <c r="T24">
         <v>-3.0521895668100615E-5</v>
       </c>
-      <c r="U24" s="25">
+      <c r="U24">
         <v>-4.7600812262649602E-6</v>
       </c>
-      <c r="V24" s="25">
+      <c r="V24">
         <v>8.1765511882469477E-5</v>
       </c>
-      <c r="W24" s="25">
+      <c r="W24">
         <v>9.4564107242971378E-5</v>
       </c>
-      <c r="X24" s="25">
+      <c r="X24">
         <v>1.8382991246653726E-5</v>
       </c>
-      <c r="Y24" s="25">
+      <c r="Y24">
         <v>4.5216905091776519E-5</v>
       </c>
-      <c r="Z24" s="25">
+      <c r="Z24">
         <v>-1.2948756174171044E-3</v>
       </c>
     </row>
@@ -8742,87 +8717,81 @@
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25">
         <v>8.2732668862811209</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25">
         <v>-2.4255406679104512E-3</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25">
         <v>-3.0680510027793956E-2</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25">
         <v>5.6750877986327768E-4</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25">
         <v>-7.3239673226412477E-3</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25">
         <v>-1.3304483028293707E-2</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25">
         <v>-1.8810521777396921E-2</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25">
         <v>-1.000691154754238E-2</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25">
         <v>-2.1529799454289289E-3</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25">
         <v>4.6194632338603658E-3</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25">
         <v>-2.6379093618582213E-3</v>
       </c>
-      <c r="M25" s="25">
+      <c r="M25">
         <v>-1.0060455310436799E-2</v>
       </c>
-      <c r="N25" s="25">
+      <c r="N25">
         <v>-1.3951013782035355E-3</v>
       </c>
-      <c r="O25" s="25">
+      <c r="O25">
         <v>-1.0453845533536895E-2</v>
       </c>
-      <c r="P25" s="25">
+      <c r="P25">
         <v>-4.5471328425719208E-3</v>
       </c>
-      <c r="Q25" s="25">
+      <c r="Q25">
         <v>-3.4379843861617326E-3</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R25">
         <v>-4.0828555161821281E-3</v>
       </c>
-      <c r="S25" s="25">
+      <c r="S25">
         <v>-2.4204761063953001E-3</v>
       </c>
-      <c r="T25" s="25">
+      <c r="T25">
         <v>-6.312444501618962E-3</v>
       </c>
-      <c r="U25" s="25">
+      <c r="U25">
         <v>-3.9597519382081475E-3</v>
       </c>
-      <c r="V25" s="25">
+      <c r="V25">
         <v>-1.1587172195334661E-2</v>
       </c>
-      <c r="W25" s="25">
+      <c r="W25">
         <v>-1.6126230233396453E-2</v>
       </c>
-      <c r="X25" s="25">
+      <c r="X25">
         <v>-4.3263767816397857E-4</v>
       </c>
-      <c r="Y25" s="25">
+      <c r="Y25">
         <v>-1.2948756174171044E-3</v>
       </c>
-      <c r="Z25" s="25">
+      <c r="Z25">
         <v>0.43353698379064198</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8831,9 +8800,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1285CCF6-ED07-4956-95C1-5161D138438C}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U21" sqref="A21:XFD22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10140,12 +10111,6 @@
       <c r="U20">
         <v>3.2956012755334996</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10173,14 +10138,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>132</v>
       </c>
     </row>
@@ -10439,16 +10404,16 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="18">
         <v>5.9691530000000004</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="18">
         <v>0.66896920000000004</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="19">
         <v>0</v>
       </c>
     </row>
@@ -10469,14 +10434,14 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="20">
         <v>3.8899999999999997E-2</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -10503,14 +10468,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>132</v>
       </c>
     </row>
@@ -10869,16 +10834,16 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="18">
         <v>8.2732670000000006</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="18">
         <v>0.65843529999999995</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="19">
         <v>0</v>
       </c>
     </row>
@@ -10899,14 +10864,14 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="20">
         <v>0.22309999999999999</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -10932,14 +10897,14 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>132</v>
       </c>
     </row>
@@ -11184,16 +11149,16 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="18">
         <v>2.4429999999999998E-4</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="18">
         <v>8.3604000000000005E-3</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="19">
         <v>0.03</v>
       </c>
     </row>
@@ -11210,16 +11175,16 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="18">
         <v>27.129180000000002</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="18">
         <v>1.8153790000000001</v>
       </c>
-      <c r="D23" s="21"/>
+      <c r="D23" s="19"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -11230,14 +11195,14 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="20">
         <v>0.3589</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>

</xml_diff>

<commit_message>
minor revisions to model parameters
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3196A4D3-8573-4042-ACCC-046101B8864B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B119E2-D677-4E69-A472-CA5E1615F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="919" activeTab="1" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="919" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -29,10 +29,18 @@
     <sheet name="IT_Process E1b - Breaks" sheetId="43" r:id="rId14"/>
     <sheet name="IT_Process E2 - Education Level" sheetId="44" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -663,9 +671,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -703,7 +711,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -809,7 +817,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -951,7 +959,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -961,9 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F25AC8-F3A4-45E4-B3D4-29D900575D65}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5586,9 +5592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED3F4A-E6FE-4140-8298-230560D8220D}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6783,9 +6787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D54BEF-A785-4097-B447-1AE751D019CE}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8802,9 +8804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1285CCF6-ED07-4956-95C1-5161D138438C}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U21" sqref="A21:XFD22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>